<commit_message>
update excel comparison model performance
</commit_message>
<xml_diff>
--- a/models/model_accuracy.xlsx
+++ b/models/model_accuracy.xlsx
@@ -1,38 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\likai\Desktop\My Life\Master\3. Semester\Innolabs\Connectome Git\models\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC60D296-B008-451A-AF42-7CD73EBBE9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05AA949C-BC70-4251-8369-9FC979A8D9E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
   <si>
     <t>Model Name</t>
   </si>
@@ -86,13 +68,127 @@
   </si>
   <si>
     <t>Aggregated by yeo7 and greater_zero</t>
+  </si>
+  <si>
+    <t>Accuracy_train</t>
+  </si>
+  <si>
+    <t>Elastic Net</t>
+  </si>
+  <si>
+    <t>conn</t>
+  </si>
+  <si>
+    <t>conn_abs</t>
+  </si>
+  <si>
+    <t>conn_squ</t>
+  </si>
+  <si>
+    <t>conn_quadratic</t>
+  </si>
+  <si>
+    <t>agg_zero</t>
+  </si>
+  <si>
+    <t>agg_max</t>
+  </si>
+  <si>
+    <t>agg_mean</t>
+  </si>
+  <si>
+    <t>gm_only</t>
+  </si>
+  <si>
+    <t>gm_conn</t>
+  </si>
+  <si>
+    <t>agg_zero_inter</t>
+  </si>
+  <si>
+    <t>agg_max_inter</t>
+  </si>
+  <si>
+    <t>agg_mean_inter</t>
+  </si>
+  <si>
+    <t>Jana</t>
+  </si>
+  <si>
+    <t>77.6</t>
+  </si>
+  <si>
+    <t>76.5</t>
+  </si>
+  <si>
+    <t>71.8</t>
+  </si>
+  <si>
+    <t>75.3</t>
+  </si>
+  <si>
+    <t>72.9</t>
+  </si>
+  <si>
+    <t>83.8</t>
+  </si>
+  <si>
+    <t>80.7</t>
+  </si>
+  <si>
+    <t>83.7</t>
+  </si>
+  <si>
+    <t>80.6</t>
+  </si>
+  <si>
+    <t>71.7</t>
+  </si>
+  <si>
+    <t>79.1</t>
+  </si>
+  <si>
+    <t>73.6</t>
+  </si>
+  <si>
+    <t>82.1</t>
+  </si>
+  <si>
+    <t>75.5</t>
+  </si>
+  <si>
+    <t>81.9</t>
+  </si>
+  <si>
+    <t>89.6</t>
+  </si>
+  <si>
+    <t>91.4</t>
+  </si>
+  <si>
+    <t>64.2</t>
+  </si>
+  <si>
+    <t>77.9</t>
+  </si>
+  <si>
+    <t>90.4</t>
+  </si>
+  <si>
+    <t>89.9</t>
+  </si>
+  <si>
+    <t>84.2</t>
+  </si>
+  <si>
+    <t>68.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +202,141 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +349,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -170,11 +572,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,11 +738,74 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="42">
+    <cellStyle name="20% - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -207,7 +820,6 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -216,7 +828,7 @@
           <bgColor rgb="FF34A853"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color rgb="FFCCCCCC"/>
@@ -228,44 +840,25 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FFCCCCCC"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{790AF9E8-5C22-4E47-8555-3FAA5356830E}" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:G20" xr:uid="{790AF9E8-5C22-4E47-8555-3FAA5356830E}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{78DCE948-4394-4ACC-8ADF-1A06A19D1601}" name="Model Name"/>
-    <tableColumn id="2" xr3:uid="{8100640F-EAF9-4641-A886-8AF3DE7E042D}" name="Architecture Design Decisions"/>
-    <tableColumn id="3" xr3:uid="{CCDFE6CD-EA1E-4337-8D4E-64AA767E86A5}" name="Datasets"/>
-    <tableColumn id="4" xr3:uid="{F3BC263A-3665-4B6A-9B77-A99BEC4EE78E}" name="Data Augmentation (Yes/No)"/>
-    <tableColumn id="5" xr3:uid="{48EDD434-876A-4AAC-9871-9CB98DAD4615}" name="Author"/>
-    <tableColumn id="6" xr3:uid="{423AAD15-5168-4DEE-812D-B88B8E0D91AD}" name="Accuracy"/>
-    <tableColumn id="7" xr3:uid="{9F7DA070-C581-4491-AE82-1AA73B74C36D}" name="AUC"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H31" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:H31">
+    <filterColumn colId="7"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Model Name"/>
+    <tableColumn id="2" name="Architecture Design Decisions"/>
+    <tableColumn id="3" name="Datasets"/>
+    <tableColumn id="4" name="Data Augmentation (Yes/No)"/>
+    <tableColumn id="5" name="Author"/>
+    <tableColumn id="6" name="Accuracy"/>
+    <tableColumn id="7" name="AUC"/>
+    <tableColumn id="8" name="Accuracy_train"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -314,7 +907,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -366,7 +959,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -560,28 +1153,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069422E6-6627-44ED-9348-7441EF273F1C}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" customWidth="1"/>
     <col min="3" max="7" width="26.77734375" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -603,8 +1197,11 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="27.6" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,7 +1224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -650,7 +1247,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,7 +1270,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="27.6" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -691,6 +1288,381 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7">
+        <v>80</v>
+      </c>
+      <c r="G8" s="7">
+        <v>80</v>
+      </c>
+      <c r="H8" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
elastic net: add model without connectivity data
</commit_message>
<xml_diff>
--- a/models/model_accuracy.xlsx
+++ b/models/model_accuracy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
   <si>
     <t>Model Name</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>68.6</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>intercept only</t>
+  </si>
+  <si>
+    <t>Elastic Net without conn</t>
+  </si>
+  <si>
+    <t>only age, sex, edyears</t>
+  </si>
+  <si>
+    <t>72.6</t>
   </si>
 </sst>
 </file>
@@ -846,8 +861,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H31" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:H31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:H33">
     <filterColumn colId="7"/>
   </autoFilter>
   <tableColumns count="8">
@@ -1153,7 +1168,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1161,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1201,58 +1216,50 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27.6" thickBot="1">
+    <row r="2" spans="1:8" ht="15" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="27.6" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1264,18 +1271,18 @@
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="27.6" thickBot="1">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -1286,76 +1293,76 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6" thickBot="1">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="7">
-        <v>100</v>
-      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="7">
-        <v>80</v>
-      </c>
-      <c r="G8" s="7">
-        <v>80</v>
-      </c>
-      <c r="H8" s="7">
-        <v>100</v>
+      <c r="F8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1">
@@ -1363,7 +1370,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1372,13 +1379,13 @@
         <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="H9" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1">
@@ -1386,7 +1393,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -1394,14 +1401,14 @@
       <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>36</v>
+      <c r="F10" s="7">
+        <v>80</v>
+      </c>
+      <c r="G10" s="7">
+        <v>80</v>
+      </c>
+      <c r="H10" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1">
@@ -1409,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -1418,13 +1425,13 @@
         <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1">
@@ -1432,7 +1439,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1441,13 +1448,13 @@
         <v>32</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1">
@@ -1455,7 +1462,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -1467,10 +1474,10 @@
         <v>35</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1">
@@ -1478,7 +1485,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1487,13 +1494,13 @@
         <v>32</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1">
@@ -1501,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -1510,13 +1517,13 @@
         <v>32</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1">
@@ -1524,7 +1531,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -1533,13 +1540,13 @@
         <v>32</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1">
@@ -1547,7 +1554,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -1559,29 +1566,57 @@
         <v>36</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H19" s="7">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="5"/>
@@ -1664,6 +1699,24 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update results elastic net
</commit_message>
<xml_diff>
--- a/models/model_accuracy.xlsx
+++ b/models/model_accuracy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
   <si>
     <t>Model Name</t>
   </si>
@@ -115,75 +115,18 @@
     <t>Jana</t>
   </si>
   <si>
-    <t>77.6</t>
-  </si>
-  <si>
-    <t>76.5</t>
-  </si>
-  <si>
     <t>71.8</t>
   </si>
   <si>
-    <t>75.3</t>
-  </si>
-  <si>
     <t>72.9</t>
   </si>
   <si>
-    <t>83.8</t>
-  </si>
-  <si>
-    <t>80.7</t>
-  </si>
-  <si>
-    <t>83.7</t>
-  </si>
-  <si>
-    <t>80.6</t>
-  </si>
-  <si>
-    <t>71.7</t>
-  </si>
-  <si>
-    <t>79.1</t>
-  </si>
-  <si>
     <t>73.6</t>
   </si>
   <si>
-    <t>82.1</t>
-  </si>
-  <si>
-    <t>75.5</t>
-  </si>
-  <si>
-    <t>81.9</t>
-  </si>
-  <si>
-    <t>89.6</t>
-  </si>
-  <si>
-    <t>91.4</t>
-  </si>
-  <si>
-    <t>64.2</t>
-  </si>
-  <si>
-    <t>77.9</t>
-  </si>
-  <si>
-    <t>90.4</t>
-  </si>
-  <si>
     <t>89.9</t>
   </si>
   <si>
-    <t>84.2</t>
-  </si>
-  <si>
-    <t>68.6</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -196,7 +139,82 @@
     <t>only age, sex, edyears</t>
   </si>
   <si>
+    <t>68.2</t>
+  </si>
+  <si>
+    <t>72.4</t>
+  </si>
+  <si>
+    <t>69.4</t>
+  </si>
+  <si>
+    <t>67.1</t>
+  </si>
+  <si>
+    <t>64.7</t>
+  </si>
+  <si>
+    <t>63.5</t>
+  </si>
+  <si>
+    <t>70.6</t>
+  </si>
+  <si>
+    <t>79.2</t>
+  </si>
+  <si>
     <t>72.6</t>
+  </si>
+  <si>
+    <t>78.9</t>
+  </si>
+  <si>
+    <t>78.3</t>
+  </si>
+  <si>
+    <t>78.1</t>
+  </si>
+  <si>
+    <t>70.1</t>
+  </si>
+  <si>
+    <t>74.2</t>
+  </si>
+  <si>
+    <t>67.7</t>
+  </si>
+  <si>
+    <t>76.7</t>
+  </si>
+  <si>
+    <t>80.3</t>
+  </si>
+  <si>
+    <t>90.9</t>
+  </si>
+  <si>
+    <t>95.8</t>
+  </si>
+  <si>
+    <t>96.4</t>
+  </si>
+  <si>
+    <t>73.2</t>
+  </si>
+  <si>
+    <t>73.8</t>
+  </si>
+  <si>
+    <t>75.1</t>
+  </si>
+  <si>
+    <t>68.3</t>
+  </si>
+  <si>
+    <t>72.2</t>
+  </si>
+  <si>
+    <t>78.2</t>
   </si>
 </sst>
 </file>
@@ -739,7 +757,7 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -761,6 +779,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1178,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1218,10 +1239,10 @@
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -1235,10 +1256,10 @@
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="15" thickBot="1">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -1248,10 +1269,10 @@
         <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="27.6" thickBot="1">
@@ -1355,14 +1376,14 @@
       <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>33</v>
+      <c r="F8" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1">
@@ -1378,14 +1399,14 @@
       <c r="E9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>33</v>
+      <c r="F9" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="7">
-        <v>100</v>
+        <v>49</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1">
@@ -1401,14 +1422,14 @@
       <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7">
-        <v>80</v>
-      </c>
-      <c r="G10" s="7">
-        <v>80</v>
-      </c>
-      <c r="H10" s="7">
-        <v>100</v>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1">
@@ -1424,14 +1445,14 @@
       <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>34</v>
+      <c r="F11" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1">
@@ -1447,14 +1468,14 @@
       <c r="E12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>34</v>
+      <c r="F12" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1">
@@ -1470,14 +1491,14 @@
       <c r="E13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>35</v>
+      <c r="F13" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1">
@@ -1493,14 +1514,14 @@
       <c r="E14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>36</v>
+      <c r="F14" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1">
@@ -1516,14 +1537,14 @@
       <c r="E15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>35</v>
+      <c r="F15" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1">
@@ -1539,14 +1560,14 @@
       <c r="E16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>33</v>
+      <c r="F16" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1">
@@ -1562,14 +1583,14 @@
       <c r="E17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>36</v>
+      <c r="F17" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="H17" s="7">
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1">
@@ -1585,14 +1606,14 @@
       <c r="E18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>37</v>
+      <c r="F18" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1">
@@ -1608,14 +1629,14 @@
       <c r="E19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="7">
-        <v>94</v>
+      <c r="F19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="7">
+        <v>75</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8">

</xml_diff>